<commit_message>
Some requisition files added
</commit_message>
<xml_diff>
--- a/Documentation STUFF/Coding Progress.xlsx
+++ b/Documentation STUFF/Coding Progress.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Noguera\Downloads\IRE_Project\IRE_Project\Documentation STUFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6EF5A6-4F9C-4358-8C40-8531CBAF7201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB3B1DD-F0E3-44F3-B5FF-BF78BFB36E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{18AC28FD-3604-45DC-800D-B8EC8976960E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{18AC28FD-3604-45DC-800D-B8EC8976960E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Code Parts" sheetId="1" r:id="rId1"/>
+    <sheet name="Methods Required" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="57">
   <si>
     <t>Controller</t>
   </si>
@@ -199,9 +199,6 @@
   </si>
   <si>
     <t>Columna1</t>
-  </si>
-  <si>
-    <t>4.5.- Update_Requisition ( as Updated)</t>
   </si>
   <si>
     <t>Metodos del API</t>
@@ -285,7 +282,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -297,6 +293,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -315,31 +314,28 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="18"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <name val="Calibri"/>
+        <name val="Century Gothic"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
       </font>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="18"/>
+        <sz val="14"/>
         <color theme="1"/>
-        <name val="Calibri"/>
+        <name val="Century Gothic"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -437,18 +433,22 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="14"/>
+        <sz val="18"/>
         <color theme="1"/>
-        <name val="Century Gothic"/>
+        <name val="Calibri"/>
         <family val="2"/>
-        <scheme val="none"/>
+        <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -461,13 +461,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="18"/>
         <color theme="1"/>
-        <name val="Century Gothic"/>
+        <name val="Calibri"/>
         <family val="2"/>
-        <scheme val="none"/>
+        <scheme val="minor"/>
       </font>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -483,7 +482,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{264791F1-49BB-4CA7-89FA-9085626E5FF4}" name="Tabla4" displayName="Tabla4" ref="B2:F11" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{264791F1-49BB-4CA7-89FA-9085626E5FF4}" name="Tabla4" displayName="Tabla4" ref="B2:F11" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="B2:F11" xr:uid="{264791F1-49BB-4CA7-89FA-9085626E5FF4}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{61C31404-3C3A-406D-95D0-C30B0B0491D8}" name="Columna1" dataDxfId="6"/>
@@ -497,10 +496,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3C99AB6-5D2A-468E-9F07-B2FD1F5EAE8C}" name="Tabla3" displayName="Tabla3" ref="B3:E48" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="B3:E48" xr:uid="{D3C99AB6-5D2A-468E-9F07-B2FD1F5EAE8C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3C99AB6-5D2A-468E-9F07-B2FD1F5EAE8C}" name="Tabla3" displayName="Tabla3" ref="B3:E47" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="B3:E47" xr:uid="{D3C99AB6-5D2A-468E-9F07-B2FD1F5EAE8C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0733E512-8498-4147-BBF9-77C5ABD974CF}" name="Metodos del API" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{0733E512-8498-4147-BBF9-77C5ABD974CF}" name="Metodos del API" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{A6A254C7-5DD0-44C7-A787-EF27655820DB}" name="Raw Code"/>
     <tableColumn id="3" xr3:uid="{62EDD18A-6580-4EE6-B67B-B7529E32A16F}" name="Verified"/>
     <tableColumn id="4" xr3:uid="{FEEC059D-286F-4D34-BC03-FF1357AAD932}" name="Validated Code"/>
@@ -808,16 +807,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63F0709-2F4D-4EBD-91AD-A821D3D193A6}">
   <dimension ref="B2:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -928,8 +927,12 @@
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
@@ -952,10 +955,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C1C583-1A41-4DE4-8755-885881DFB974}">
-  <dimension ref="B3:E48"/>
+  <dimension ref="B3:E47"/>
   <sheetViews>
-    <sheetView zoomScale="78" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="78" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,16 +970,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1020,11 +1023,11 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="2:5" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+    <row r="9" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
@@ -1086,7 +1089,7 @@
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -1096,10 +1099,10 @@
       <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1107,10 +1110,10 @@
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="C17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1118,10 +1121,10 @@
       <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="12" t="s">
+      <c r="C18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1129,10 +1132,10 @@
       <c r="B19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="12" t="s">
+      <c r="C19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1140,14 +1143,14 @@
       <c r="B20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -1162,202 +1165,210 @@
       <c r="B23" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
     </row>
     <row r="24" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C24" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" t="s">
-        <v>57</v>
+      <c r="C24" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B28" s="5" t="s">
+      <c r="C25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B27" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+    </row>
+    <row r="28" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+    </row>
+    <row r="29" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B29" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
     </row>
     <row r="30" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B31" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="6"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" t="s">
-        <v>12</v>
+        <v>39</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" t="s">
-        <v>56</v>
+        <v>40</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
+      <c r="C37" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="6"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="40" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" t="s">
-        <v>12</v>
-      </c>
-      <c r="D41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" t="s">
-        <v>12</v>
-      </c>
-      <c r="D42" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C43" t="s">
-        <v>12</v>
-      </c>
-      <c r="D43" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
+      <c r="C42" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="6"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B44" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
     </row>
     <row r="45" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B48" s="3" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dish - Verified Code
</commit_message>
<xml_diff>
--- a/Documentation STUFF/Coding Progress.xlsx
+++ b/Documentation STUFF/Coding Progress.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Noguera\Downloads\IRE_Project\IRE_Project\Documentation STUFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Noguera\Documents\IRE_PROJECT\Documentation STUFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB3B1DD-F0E3-44F3-B5FF-BF78BFB36E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE1F5ED-15EE-4533-9C53-DA1C8E785B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{18AC28FD-3604-45DC-800D-B8EC8976960E}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{18AC28FD-3604-45DC-800D-B8EC8976960E}"/>
   </bookViews>
   <sheets>
     <sheet name="Code Parts" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="57">
   <si>
     <t>Controller</t>
   </si>
@@ -482,8 +482,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{264791F1-49BB-4CA7-89FA-9085626E5FF4}" name="Tabla4" displayName="Tabla4" ref="B2:F11" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="B2:F11" xr:uid="{264791F1-49BB-4CA7-89FA-9085626E5FF4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{264791F1-49BB-4CA7-89FA-9085626E5FF4}" name="Tabla4" displayName="Tabla4" ref="B2:F10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="B2:F10" xr:uid="{264791F1-49BB-4CA7-89FA-9085626E5FF4}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{61C31404-3C3A-406D-95D0-C30B0B0491D8}" name="Columna1" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{00A67C08-5D98-4E74-93D5-0FDEABBB7F9A}" name="Model" dataDxfId="5"/>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63F0709-2F4D-4EBD-91AD-A821D3D193A6}">
   <dimension ref="B2:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,7 +817,7 @@
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -875,10 +875,18 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
@@ -933,8 +941,12 @@
       <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
@@ -957,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C1C583-1A41-4DE4-8755-885881DFB974}">
   <dimension ref="B3:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="78" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,7 +999,9 @@
       <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
@@ -995,32 +1009,48 @@
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -1160,12 +1190,20 @@
       <c r="B22" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="C22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="23" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="D23" s="11"/>
     </row>
     <row r="24" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Recipe Raw Code - SQL Queries started
</commit_message>
<xml_diff>
--- a/Documentation STUFF/Coding Progress.xlsx
+++ b/Documentation STUFF/Coding Progress.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Noguera\Documents\IRE_PROJECT\Documentation STUFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Noguera\Downloads\IRE_Project\IRE_Project\Documentation STUFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE1F5ED-15EE-4533-9C53-DA1C8E785B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23BD720-B5A2-4D05-93EE-8D7903490B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{18AC28FD-3604-45DC-800D-B8EC8976960E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{18AC28FD-3604-45DC-800D-B8EC8976960E}"/>
   </bookViews>
   <sheets>
     <sheet name="Code Parts" sheetId="1" r:id="rId1"/>
     <sheet name="Methods Required" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="59">
   <si>
     <t>Controller</t>
   </si>
@@ -208,6 +209,12 @@
   </si>
   <si>
     <t>pend</t>
+  </si>
+  <si>
+    <t>Add_Ingredients:</t>
+  </si>
+  <si>
+    <t>JOINS</t>
   </si>
 </sst>
 </file>
@@ -496,8 +503,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3C99AB6-5D2A-468E-9F07-B2FD1F5EAE8C}" name="Tabla3" displayName="Tabla3" ref="B3:E47" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="B3:E47" xr:uid="{D3C99AB6-5D2A-468E-9F07-B2FD1F5EAE8C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3C99AB6-5D2A-468E-9F07-B2FD1F5EAE8C}" name="Tabla3" displayName="Tabla3" ref="B3:E48" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="B3:E48" xr:uid="{D3C99AB6-5D2A-468E-9F07-B2FD1F5EAE8C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0733E512-8498-4147-BBF9-77C5ABD974CF}" name="Metodos del API" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{A6A254C7-5DD0-44C7-A787-EF27655820DB}" name="Raw Code"/>
@@ -967,10 +974,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C1C583-1A41-4DE4-8755-885881DFB974}">
-  <dimension ref="B3:E47"/>
+  <dimension ref="B3:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,52 +1243,47 @@
     </row>
     <row r="27" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
     </row>
-    <row r="28" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>35</v>
+    <row r="28" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
     </row>
-    <row r="29" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B29" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="11"/>
+    <row r="29" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="D29" s="11"/>
     </row>
     <row r="30" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>12</v>
-      </c>
+    <row r="31" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="6"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="6"/>
     </row>
     <row r="33" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>12</v>
@@ -1292,27 +1294,27 @@
     </row>
     <row r="34" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="11"/>
+        <v>38</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="D34" s="11" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>12</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C35" s="11"/>
       <c r="D35" s="11" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>12</v>
@@ -1323,35 +1325,35 @@
     </row>
     <row r="37" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="6"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="6"/>
-    </row>
-    <row r="39" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>12</v>
-      </c>
+      <c r="C38" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="6"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="6"/>
     </row>
     <row r="40" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>12</v>
@@ -1362,7 +1364,7 @@
     </row>
     <row r="41" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>12</v>
@@ -1373,40 +1375,51 @@
     </row>
     <row r="42" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="6"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B44" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
+      <c r="C43" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="6"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="6"/>
     </row>
     <row r="45" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>49</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
     </row>
     <row r="46" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B48" s="3" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1417,4 +1430,24 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A47B49-C914-43CD-890D-24379F1240F4}">
+  <dimension ref="C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Some of the biggest recipe methods are joined
</commit_message>
<xml_diff>
--- a/Documentation STUFF/Coding Progress.xlsx
+++ b/Documentation STUFF/Coding Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Noguera\Downloads\IRE_Project\IRE_Project\Documentation STUFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23BD720-B5A2-4D05-93EE-8D7903490B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4444EA1-F0A9-4EB4-ABA5-72B2DCDEB7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{18AC28FD-3604-45DC-800D-B8EC8976960E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{18AC28FD-3604-45DC-800D-B8EC8976960E}"/>
   </bookViews>
   <sheets>
     <sheet name="Code Parts" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="59">
   <si>
     <t>Controller</t>
   </si>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C1C583-1A41-4DE4-8755-885881DFB974}">
   <dimension ref="B3:E48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1211,9 @@
       <c r="C23" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="11"/>
+      <c r="D23" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="24" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
@@ -1245,35 +1247,56 @@
       <c r="B27" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
+      <c r="C27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="28" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
+      <c r="C28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="11"/>
+      <c r="C29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="30" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
+      <c r="C30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
+      <c r="C31" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
@@ -1436,7 +1459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A47B49-C914-43CD-890D-24379F1240F4}">
   <dimension ref="C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Movement Raw Code - Completed
</commit_message>
<xml_diff>
--- a/Documentation STUFF/Coding Progress.xlsx
+++ b/Documentation STUFF/Coding Progress.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Noguera\Downloads\IRE_Project\IRE_Project\Documentation STUFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Noguera\Documents\IRE_PROJECT\Documentation STUFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9164535-6D88-4743-9D72-A4FFF7A94AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD77172C-4D2F-46D4-8B08-2B61456B2139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{18AC28FD-3604-45DC-800D-B8EC8976960E}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{18AC28FD-3604-45DC-800D-B8EC8976960E}"/>
   </bookViews>
   <sheets>
     <sheet name="Code Parts" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="59">
   <si>
     <t>Controller</t>
   </si>
@@ -974,10 +974,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C1C583-1A41-4DE4-8755-885881DFB974}">
-  <dimension ref="B3:E48"/>
+  <dimension ref="B3:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1430,23 +1430,37 @@
       <c r="B45" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="11"/>
+      <c r="C45" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="D45" s="11"/>
     </row>
     <row r="46" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="C46" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="47" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="C47" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="48" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="C48" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Movement Controller - Completed
</commit_message>
<xml_diff>
--- a/Documentation STUFF/Coding Progress.xlsx
+++ b/Documentation STUFF/Coding Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Noguera\Documents\IRE_PROJECT\Documentation STUFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD77172C-4D2F-46D4-8B08-2B61456B2139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C525A92F-F68E-44FB-84CA-3E9784741E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{18AC28FD-3604-45DC-800D-B8EC8976960E}"/>
+    <workbookView xWindow="25365" yWindow="0" windowWidth="18900" windowHeight="10140" activeTab="1" xr2:uid="{18AC28FD-3604-45DC-800D-B8EC8976960E}"/>
   </bookViews>
   <sheets>
     <sheet name="Code Parts" sheetId="1" r:id="rId1"/>
@@ -977,7 +977,7 @@
   <dimension ref="B3:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ACTUALIZATION DB - All dish Bridge Model Completed!
</commit_message>
<xml_diff>
--- a/Documentation STUFF/Coding Progress.xlsx
+++ b/Documentation STUFF/Coding Progress.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio Noguera\Documents\IRE_PROJECT\Documentation STUFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C525A92F-F68E-44FB-84CA-3E9784741E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF9DF66-AA29-4C1F-A608-804B4464E4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25365" yWindow="0" windowWidth="18900" windowHeight="10140" activeTab="1" xr2:uid="{18AC28FD-3604-45DC-800D-B8EC8976960E}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{18AC28FD-3604-45DC-800D-B8EC8976960E}"/>
   </bookViews>
   <sheets>
     <sheet name="Code Parts" sheetId="1" r:id="rId1"/>
     <sheet name="Methods Required" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
+    <sheet name="Validation Required" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="60">
   <si>
     <t>Controller</t>
   </si>
@@ -215,6 +216,9 @@
   </si>
   <si>
     <t>JOINS</t>
+  </si>
+  <si>
+    <t>Complejidad(#Pruebas)</t>
   </si>
 </sst>
 </file>
@@ -309,7 +313,41 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -489,27 +527,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{264791F1-49BB-4CA7-89FA-9085626E5FF4}" name="Tabla4" displayName="Tabla4" ref="B2:F10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{264791F1-49BB-4CA7-89FA-9085626E5FF4}" name="Tabla4" displayName="Tabla4" ref="B2:F10" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="B2:F10" xr:uid="{264791F1-49BB-4CA7-89FA-9085626E5FF4}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{61C31404-3C3A-406D-95D0-C30B0B0491D8}" name="Columna1" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00A67C08-5D98-4E74-93D5-0FDEABBB7F9A}" name="Model" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{73698F15-06A7-4753-B3FF-D764E1A49ECE}" name="Repositories" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{FE5779E4-8E44-48CB-A152-64B2D7C38C9F}" name="Service" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{50A140DE-1488-476E-AACA-7F19CE60D9DF}" name="Controller" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{61C31404-3C3A-406D-95D0-C30B0B0491D8}" name="Columna1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00A67C08-5D98-4E74-93D5-0FDEABBB7F9A}" name="Model" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{73698F15-06A7-4753-B3FF-D764E1A49ECE}" name="Repositories" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{FE5779E4-8E44-48CB-A152-64B2D7C38C9F}" name="Service" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{50A140DE-1488-476E-AACA-7F19CE60D9DF}" name="Controller" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3C99AB6-5D2A-468E-9F07-B2FD1F5EAE8C}" name="Tabla3" displayName="Tabla3" ref="B3:E48" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D3C99AB6-5D2A-468E-9F07-B2FD1F5EAE8C}" name="Tabla3" displayName="Tabla3" ref="B3:E48" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="B3:E48" xr:uid="{D3C99AB6-5D2A-468E-9F07-B2FD1F5EAE8C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0733E512-8498-4147-BBF9-77C5ABD974CF}" name="Metodos del API" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0733E512-8498-4147-BBF9-77C5ABD974CF}" name="Metodos del API" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{A6A254C7-5DD0-44C7-A787-EF27655820DB}" name="Raw Code"/>
     <tableColumn id="3" xr3:uid="{62EDD18A-6580-4EE6-B67B-B7529E32A16F}" name="Verified"/>
     <tableColumn id="4" xr3:uid="{FEEC059D-286F-4D34-BC03-FF1357AAD932}" name="Validated Code"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{150E0BF6-9944-43B3-8D94-CB571CF38092}" name="Tabla32" displayName="Tabla32" ref="B3:C48" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="B3:C48" xr:uid="{D3C99AB6-5D2A-468E-9F07-B2FD1F5EAE8C}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{38DC75B2-1B28-4D59-A8E0-0D69C96C4FCE}" name="Metodos del API" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{C2A96D02-52CA-42FB-B70D-DE602BF3CF3D}" name="Complejidad(#Pruebas)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -976,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63C1C583-1A41-4DE4-8755-885881DFB974}">
   <dimension ref="B3:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,4 +1538,294 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C45F06-FE13-4860-A8EE-13C826069465}">
+  <dimension ref="B3:C49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="11"/>
+    </row>
+    <row r="19" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="11"/>
+    </row>
+    <row r="25" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="11"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="12"/>
+    </row>
+    <row r="27" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B27" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="11"/>
+    </row>
+    <row r="28" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="11"/>
+    </row>
+    <row r="29" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="11"/>
+    </row>
+    <row r="30" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B30" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="11"/>
+    </row>
+    <row r="31" spans="2:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="11"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="6"/>
+      <c r="C32" s="12"/>
+    </row>
+    <row r="33" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="11"/>
+    </row>
+    <row r="34" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="11"/>
+    </row>
+    <row r="35" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="11"/>
+    </row>
+    <row r="36" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="11"/>
+    </row>
+    <row r="37" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="11"/>
+    </row>
+    <row r="38" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="11"/>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="6"/>
+      <c r="C39" s="12"/>
+    </row>
+    <row r="40" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="11"/>
+    </row>
+    <row r="41" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="11"/>
+    </row>
+    <row r="42" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="11"/>
+    </row>
+    <row r="43" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="11"/>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="6"/>
+      <c r="C44" s="12"/>
+    </row>
+    <row r="45" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B45" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="11"/>
+    </row>
+    <row r="46" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="11"/>
+    </row>
+    <row r="47" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B47" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="11"/>
+    </row>
+    <row r="48" spans="2:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B48" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="11"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>